<commit_message>
modified the V2 left_arm and right_arm visualization.
svn path=/trunk/iCub/; revision=23848
</commit_message>
<xml_diff>
--- a/app/skinGui/iniGenerators/leftArm_ini_generator iCubV2.xlsx
+++ b/app/skinGui/iniGenerators/leftArm_ini_generator iCubV2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="12570" yWindow="-270" windowWidth="12600" windowHeight="12975" activeTab="4"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12600" windowHeight="12000" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="lower" sheetId="1" r:id="rId1"/>
@@ -2016,8 +2016,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10250287" y="0"/>
-          <a:ext cx="4028311" cy="0"/>
+          <a:off x="10251799" y="0"/>
+          <a:ext cx="4023775" cy="0"/>
           <a:chOff x="10981462" y="1799664"/>
           <a:chExt cx="5588677" cy="4621561"/>
         </a:xfrm>
@@ -3040,8 +3040,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10239703" y="2320295"/>
-          <a:ext cx="4365297" cy="3716062"/>
+          <a:off x="10236679" y="2327855"/>
+          <a:ext cx="4365297" cy="3719085"/>
           <a:chOff x="10968014" y="1847464"/>
           <a:chExt cx="5518210" cy="4625913"/>
         </a:xfrm>
@@ -5097,8 +5097,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10768870" y="0"/>
-          <a:ext cx="4038894" cy="0"/>
+          <a:off x="10740855" y="0"/>
+          <a:ext cx="4030179" cy="0"/>
           <a:chOff x="10981462" y="1799664"/>
           <a:chExt cx="5588677" cy="4621561"/>
         </a:xfrm>
@@ -6121,8 +6121,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10726537" y="2320295"/>
-          <a:ext cx="4397046" cy="3716062"/>
+          <a:off x="10698522" y="2324653"/>
+          <a:ext cx="4388331" cy="3716684"/>
           <a:chOff x="10968014" y="1847464"/>
           <a:chExt cx="5518210" cy="4625913"/>
         </a:xfrm>
@@ -8214,8 +8214,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10705370" y="0"/>
-          <a:ext cx="4038894" cy="0"/>
+          <a:off x="10684826" y="0"/>
+          <a:ext cx="4030179" cy="0"/>
           <a:chOff x="10981462" y="1799664"/>
           <a:chExt cx="5588677" cy="4621561"/>
         </a:xfrm>
@@ -9238,8 +9238,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10663037" y="2320295"/>
-          <a:ext cx="4524046" cy="3716062"/>
+          <a:off x="10642493" y="2324653"/>
+          <a:ext cx="4515331" cy="3716684"/>
           <a:chOff x="10968014" y="1847464"/>
           <a:chExt cx="5518210" cy="4625913"/>
         </a:xfrm>
@@ -11350,8 +11350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T55"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11466,7 +11466,7 @@
         <v>16</v>
       </c>
       <c r="R3" s="56">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="T3" s="21" t="s">
         <v>18</v>
@@ -11482,7 +11482,7 @@
       </c>
       <c r="C4" s="71">
         <f>((+O4*COS($N$3)-P4*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-103.92225100748811</v>
+        <v>-67.077748992511886</v>
       </c>
       <c r="D4" s="71">
         <f>((O4*SIN($N$3)+P4*COS($N$3)+$N$9)*$R$4)</f>
@@ -11490,14 +11490,14 @@
       </c>
       <c r="E4" s="71">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M4/3.1416*180)+$N$5)</f>
-        <v>-89.999859694228434</v>
+        <v>89.999859694228434</v>
       </c>
       <c r="F4" s="70">
         <v>5</v>
       </c>
       <c r="G4" s="73">
-        <f t="shared" ref="G3:G7" si="1">IF($R$3*$R$4=-1,1,0)</f>
-        <v>0</v>
+        <f t="shared" ref="G4:G7" si="1">IF($R$3*$R$4=-1,1,0)</f>
+        <v>1</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -11540,7 +11540,7 @@
       </c>
       <c r="C5" s="71">
         <f>((+O5*COS($N$3)-P5*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-94.684646700454095</v>
+        <v>-76.315353299545905</v>
       </c>
       <c r="D5" s="71">
         <f>((O5*SIN($N$3)+P5*COS($N$3)+$N$9)*$R$4)</f>
@@ -11548,14 +11548,14 @@
       </c>
       <c r="E5" s="71">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M5/3.1416*180)+$N$5)</f>
-        <v>-149.99971938845687</v>
+        <v>149.99971938845687</v>
       </c>
       <c r="F5" s="70">
         <v>5</v>
       </c>
       <c r="G5" s="73">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -11597,7 +11597,7 @@
       </c>
       <c r="C6" s="71">
         <f>((+O6*COS($N$3)-P6*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-76.209438086386058</v>
+        <v>-94.790561913613942</v>
       </c>
       <c r="D6" s="71">
         <f>((O6*SIN($N$3)+P6*COS($N$3)+$N$9)*$R$4)</f>
@@ -11605,14 +11605,14 @@
       </c>
       <c r="E6" s="71">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M6/3.1416*180)+$N$5)</f>
-        <v>-89.999859694228434</v>
+        <v>89.999859694228434</v>
       </c>
       <c r="F6" s="70">
         <v>5</v>
       </c>
       <c r="G6" s="73">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -11652,7 +11652,7 @@
       </c>
       <c r="C7" s="71">
         <f>((+O7*COS($N$3)-P7*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-66.971833779352067</v>
+        <v>-104.02816622064793</v>
       </c>
       <c r="D7" s="71">
         <f>((O7*SIN($N$3)+P7*COS($N$3)+$N$9)*$R$4)</f>
@@ -11660,14 +11660,14 @@
       </c>
       <c r="E7" s="71">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M7/3.1416*180)+$N$5)</f>
-        <v>-30</v>
+        <v>30</v>
       </c>
       <c r="F7" s="70">
         <v>5</v>
       </c>
       <c r="G7" s="73">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -11684,7 +11684,7 @@
         <v>0</v>
       </c>
       <c r="N7" s="3">
-        <v>-259</v>
+        <v>-88</v>
       </c>
       <c r="O7" s="46">
         <v>148</v>
@@ -11804,7 +11804,7 @@
       </c>
       <c r="C11" s="71">
         <f t="shared" ref="C11:C14" si="4">((+O11*COS($N$3)-P11*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-94.684646700454124</v>
+        <v>-76.315353299545876</v>
       </c>
       <c r="D11" s="71">
         <f t="shared" ref="D11:D14" si="5">((O11*SIN($N$3)+P11*COS($N$3)+$N$9)*$R$4)</f>
@@ -11812,14 +11812,14 @@
       </c>
       <c r="E11" s="71">
         <f t="shared" ref="E11:E14" si="6">IF(($R$3*$R$4)=1,1,-1)*(($M11/3.1416*180)+$N$5)</f>
-        <v>-30</v>
+        <v>30</v>
       </c>
       <c r="F11" s="70">
         <v>5</v>
       </c>
       <c r="G11" s="73">
         <f t="shared" ref="G11:G14" si="7">IF($R$3*$R$4=-1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="45">
@@ -11854,7 +11854,7 @@
       </c>
       <c r="C12" s="71">
         <f t="shared" si="4"/>
-        <v>-76.209438086386115</v>
+        <v>-94.790561913613885</v>
       </c>
       <c r="D12" s="71">
         <f t="shared" si="5"/>
@@ -11862,14 +11862,14 @@
       </c>
       <c r="E12" s="71">
         <f t="shared" si="6"/>
-        <v>-89.999859694228434</v>
+        <v>89.999859694228434</v>
       </c>
       <c r="F12" s="70">
         <v>5</v>
       </c>
       <c r="G12" s="73">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="45">
@@ -11902,7 +11902,7 @@
       </c>
       <c r="C13" s="71">
         <f t="shared" si="4"/>
-        <v>-66.971833779352096</v>
+        <v>-104.0281662206479</v>
       </c>
       <c r="D13" s="71">
         <f t="shared" si="5"/>
@@ -11910,14 +11910,14 @@
       </c>
       <c r="E13" s="71">
         <f t="shared" si="6"/>
-        <v>-30</v>
+        <v>30</v>
       </c>
       <c r="F13" s="70">
         <v>5</v>
       </c>
       <c r="G13" s="73">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="45">
@@ -11950,7 +11950,7 @@
       </c>
       <c r="C14" s="71">
         <f t="shared" si="4"/>
-        <v>-76.209438086386115</v>
+        <v>-94.790561913613885</v>
       </c>
       <c r="D14" s="71">
         <f t="shared" si="5"/>
@@ -11958,14 +11958,14 @@
       </c>
       <c r="E14" s="71">
         <f t="shared" si="6"/>
-        <v>29.999859694228427</v>
+        <v>-29.999859694228427</v>
       </c>
       <c r="F14" s="70">
         <v>5</v>
       </c>
       <c r="G14" s="73">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="45">
@@ -12114,7 +12114,7 @@
       </c>
       <c r="C19" s="71">
         <f>((+O19*COS($N$3)-P19*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-94.684646700454152</v>
+        <v>-76.315353299545848</v>
       </c>
       <c r="D19" s="71">
         <f>((O19*SIN($N$3)+P19*COS($N$3)+$N$9)*$R$4)</f>
@@ -12122,14 +12122,14 @@
       </c>
       <c r="E19" s="71">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M19/3.1416*180)+$N$5)</f>
-        <v>89.999719388456853</v>
+        <v>-89.999719388456853</v>
       </c>
       <c r="F19" s="70">
         <v>5</v>
       </c>
       <c r="G19" s="73">
         <f t="shared" ref="G19" si="9">IF($R$3*$R$4=-1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="45">
@@ -12244,27 +12244,27 @@
         <v>26</v>
       </c>
       <c r="B23" s="71">
-        <f t="shared" ref="B23:B25" si="10">((ROUND($L23/10,0))-1)*4+MOD($L23,10)+((J23-1)*16)</f>
+        <f t="shared" ref="B23" si="10">((ROUND($L23/10,0))-1)*4+MOD($L23,10)+((J23-1)*16)</f>
         <v>11</v>
       </c>
       <c r="C23" s="71">
-        <f t="shared" ref="C23:C25" si="11">((+O23*COS($N$3)-P23*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-103.92225100748814</v>
+        <f t="shared" ref="C23" si="11">((+O23*COS($N$3)-P23*SIN($N$3)+$N$7)*$R$3)</f>
+        <v>-67.077748992511857</v>
       </c>
       <c r="D23" s="71">
-        <f t="shared" ref="D23:D25" si="12">((O23*SIN($N$3)+P23*COS($N$3)+$N$9)*$R$4)</f>
+        <f t="shared" ref="D23" si="12">((O23*SIN($N$3)+P23*COS($N$3)+$N$9)*$R$4)</f>
         <v>147.60254037844382</v>
       </c>
       <c r="E23" s="71">
-        <f t="shared" ref="E23:E25" si="13">IF(($R$3*$R$4)=1,1,-1)*(($M23/3.1416*180)+$N$5)</f>
-        <v>149.99957908268468</v>
+        <f t="shared" ref="E23" si="13">IF(($R$3*$R$4)=1,1,-1)*(($M23/3.1416*180)+$N$5)</f>
+        <v>-149.99957908268468</v>
       </c>
       <c r="F23" s="70">
         <v>5</v>
       </c>
       <c r="G23" s="73">
-        <f t="shared" ref="G23:G25" si="14">IF($R$3*$R$4=-1,1,0)</f>
-        <v>0</v>
+        <f t="shared" ref="G23" si="14">IF($R$3*$R$4=-1,1,0)</f>
+        <v>1</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="45">
@@ -12606,10 +12606,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T30"/>
+  <dimension ref="A1:T32"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12693,22 +12693,22 @@
       </c>
       <c r="C3" s="71">
         <f>((+O3*COS($N$3)-P3*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-36.602540378443848</v>
+        <v>-16.397459621556152</v>
       </c>
       <c r="D3" s="71">
         <f>((O3*SIN($N$3)+P3*COS($N$3)+$N$9)*$R$4)</f>
-        <v>161.39745962155612</v>
+        <v>163.39745962155612</v>
       </c>
       <c r="E3" s="71">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M3/3.1416*180)+$N$5)</f>
-        <v>210</v>
+        <v>-210</v>
       </c>
       <c r="F3" s="70">
         <v>5</v>
       </c>
       <c r="G3" s="73">
         <f t="shared" ref="G3:G4" si="1">IF($R$3*$R$4=-1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -12738,7 +12738,7 @@
         <v>16</v>
       </c>
       <c r="R3" s="56">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="T3" s="21" t="s">
         <v>18</v>
@@ -12754,22 +12754,22 @@
       </c>
       <c r="C4" s="71">
         <f>((+O4*COS($N$3)-P4*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-45.84014468547786</v>
+        <v>-7.1598553145221402</v>
       </c>
       <c r="D4" s="71">
         <f>((O4*SIN($N$3)+P4*COS($N$3)+$N$9)*$R$4)</f>
-        <v>145.39745962155615</v>
+        <v>147.39745962155615</v>
       </c>
       <c r="E4" s="71">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M4/3.1416*180)+$N$5)</f>
-        <v>150.00014030577157</v>
+        <v>-150.00014030577157</v>
       </c>
       <c r="F4" s="70">
         <v>5</v>
       </c>
       <c r="G4" s="73">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -12899,7 +12899,7 @@
         <v>0</v>
       </c>
       <c r="N7" s="3">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="O7" s="46">
         <v>148</v>
@@ -12968,7 +12968,7 @@
         <v>0</v>
       </c>
       <c r="N9" s="3">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="O9" s="46">
         <v>164</v>
@@ -13019,22 +13019,22 @@
       </c>
       <c r="C11" s="71">
         <f>((+O11*COS($N$3)-P11*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-36.602540378443862</v>
+        <v>-16.397459621556138</v>
       </c>
       <c r="D11" s="71">
         <f>((O11*SIN($N$3)+P11*COS($N$3)+$N$9)*$R$4)</f>
-        <v>129.39745962155615</v>
+        <v>131.39745962155615</v>
       </c>
       <c r="E11" s="71">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M11/3.1416*180)+$N$5)</f>
-        <v>210</v>
+        <v>-210</v>
       </c>
       <c r="F11" s="70">
         <v>5</v>
       </c>
       <c r="G11" s="73">
         <f t="shared" ref="G11:G15" si="3">IF($R$3*$R$4=-1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="43">
@@ -13069,22 +13069,22 @@
       </c>
       <c r="C12" s="71">
         <f>((+O12*COS($N$3)-P12*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-45.840144685477881</v>
+        <v>-7.1598553145221189</v>
       </c>
       <c r="D12" s="71">
         <f>((O12*SIN($N$3)+P12*COS($N$3)+$N$9)*$R$4)</f>
-        <v>113.39745962155618</v>
+        <v>115.39745962155618</v>
       </c>
       <c r="E12" s="71">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M12/3.1416*180)+$N$5)</f>
-        <v>150.00014030577157</v>
+        <v>-150.00014030577157</v>
       </c>
       <c r="F12" s="70">
         <v>5</v>
       </c>
       <c r="G12" s="73">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="43">
@@ -13117,22 +13117,22 @@
       </c>
       <c r="C13" s="71">
         <f>((+O13*COS($N$3)-P13*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-36.602540378443877</v>
+        <v>-16.397459621556123</v>
       </c>
       <c r="D13" s="71">
         <f>((O13*SIN($N$3)+P13*COS($N$3)+$N$9)*$R$4)</f>
-        <v>97.397459621556209</v>
+        <v>99.397459621556209</v>
       </c>
       <c r="E13" s="71">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M13/3.1416*180)+$N$5)</f>
-        <v>210</v>
+        <v>-210</v>
       </c>
       <c r="F13" s="70">
         <v>5</v>
       </c>
       <c r="G13" s="73">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="43">
@@ -13165,22 +13165,22 @@
       </c>
       <c r="C14" s="71">
         <f>((+O14*COS($N$3)-P14*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-18.127331764375867</v>
+        <v>-34.872668235624133</v>
       </c>
       <c r="D14" s="71">
         <f>((O14*SIN($N$3)+P14*COS($N$3)+$N$9)*$R$4)</f>
-        <v>97.397459621556209</v>
+        <v>99.397459621556209</v>
       </c>
       <c r="E14" s="71">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M14/3.1416*180)+$N$5)</f>
-        <v>269.99985969422841</v>
+        <v>-269.99985969422841</v>
       </c>
       <c r="F14" s="70">
         <v>5</v>
       </c>
       <c r="G14" s="73">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="43">
@@ -13213,22 +13213,22 @@
       </c>
       <c r="C15" s="71">
         <f>((+O15*COS($N$3)-P15*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-8.8897274573418628</v>
+        <v>-44.110272542658137</v>
       </c>
       <c r="D15" s="71">
         <f>((O15*SIN($N$3)+P15*COS($N$3)+$N$9)*$R$4)</f>
-        <v>81.397459621556209</v>
+        <v>83.397459621556209</v>
       </c>
       <c r="E15" s="71">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M15/3.1416*180)+$N$5)</f>
-        <v>210</v>
+        <v>-210</v>
       </c>
       <c r="F15" s="70">
         <v>5</v>
       </c>
       <c r="G15" s="73">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="43">
@@ -13280,7 +13280,7 @@
         <v>192.37604307033999</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="25"/>
       <c r="B17" s="36"/>
       <c r="C17" s="24"/>
@@ -13309,7 +13309,7 @@
         <v>192.37604307033999</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
       <c r="B18" s="36"/>
       <c r="C18" s="24"/>
@@ -13338,7 +13338,7 @@
         <v>183.138438763306</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="72" t="s">
         <v>26</v>
       </c>
@@ -13348,22 +13348,22 @@
       </c>
       <c r="C19" s="71">
         <f>((+O19*COS($N$3)-P19*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-8.8897274573418485</v>
+        <v>-44.110272542658151</v>
       </c>
       <c r="D19" s="71">
         <f>((O19*SIN($N$3)+P19*COS($N$3)+$N$9)*$R$4)</f>
-        <v>113.39745962155621</v>
+        <v>115.39745962155621</v>
       </c>
       <c r="E19" s="71">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M19/3.1416*180)+$N$5)</f>
-        <v>329.99971938845687</v>
+        <v>-329.99971938845687</v>
       </c>
       <c r="F19" s="70">
         <v>5</v>
       </c>
       <c r="G19" s="73">
         <f t="shared" ref="G19" si="5">IF($R$3*$R$4=-1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="43">
@@ -13386,7 +13386,7 @@
         <v>155.425625842204</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="25"/>
       <c r="B20" s="36"/>
       <c r="C20" s="24"/>
@@ -13415,7 +13415,7 @@
         <v>164.66323014923799</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="25"/>
       <c r="B21" s="36"/>
       <c r="C21" s="24"/>
@@ -13444,7 +13444,7 @@
         <v>155.425625842204</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="25"/>
       <c r="B22" s="36"/>
       <c r="C22" s="24"/>
@@ -13473,7 +13473,7 @@
         <v>136.95041722813599</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="72" t="s">
         <v>26</v>
       </c>
@@ -13483,22 +13483,22 @@
       </c>
       <c r="C23" s="71">
         <f>((+O23*COS($N$3)-P23*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-18.127331764375853</v>
+        <v>-34.872668235624147</v>
       </c>
       <c r="D23" s="71">
         <f>((O23*SIN($N$3)+P23*COS($N$3)+$N$9)*$R$4)</f>
-        <v>129.39745962155618</v>
+        <v>131.39745962155618</v>
       </c>
       <c r="E23" s="71">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M23/3.1416*180)+$N$5)</f>
-        <v>389.9995790826847</v>
+        <v>-389.9995790826847</v>
       </c>
       <c r="F23" s="70">
         <v>5</v>
       </c>
       <c r="G23" s="73">
         <f t="shared" ref="G23:G25" si="7">IF($R$3*$R$4=-1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="43">
@@ -13521,7 +13521,7 @@
         <v>136.95041722813599</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="72" t="s">
         <v>26</v>
       </c>
@@ -13531,22 +13531,22 @@
       </c>
       <c r="C24" s="71">
         <f>((+O24*COS($N$3)-P24*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-8.8897274573418343</v>
+        <v>-44.110272542658166</v>
       </c>
       <c r="D24" s="71">
         <f>((O24*SIN($N$3)+P24*COS($N$3)+$N$9)*$R$4)</f>
-        <v>145.39745962155618</v>
+        <v>147.39745962155618</v>
       </c>
       <c r="E24" s="71">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M24/3.1416*180)+$N$5)</f>
-        <v>329.99971938845687</v>
+        <v>-329.99971938845687</v>
       </c>
       <c r="F24" s="70">
         <v>5</v>
       </c>
       <c r="G24" s="73">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="43">
@@ -13569,7 +13569,7 @@
         <v>127.712812921102</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="72" t="s">
         <v>26</v>
       </c>
@@ -13579,22 +13579,22 @@
       </c>
       <c r="C25" s="71">
         <f>((+O25*COS($N$3)-P25*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-18.127331764375832</v>
+        <v>-34.872668235624168</v>
       </c>
       <c r="D25" s="71">
         <f>((O25*SIN($N$3)+P25*COS($N$3)+$N$9)*$R$4)</f>
-        <v>161.39745962155615</v>
+        <v>163.39745962155615</v>
       </c>
       <c r="E25" s="71">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M25/3.1416*180)+$N$5)</f>
-        <v>389.9995790826847</v>
+        <v>-389.9995790826847</v>
       </c>
       <c r="F25" s="70">
         <v>5</v>
       </c>
       <c r="G25" s="73">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="43">
@@ -13617,13 +13617,18 @@
         <v>109.237604307034</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="J26" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="N30" s="61"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T32">
+        <v>4616</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13636,8 +13641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13720,22 +13725,22 @@
       </c>
       <c r="C3" s="71">
         <f t="shared" ref="C3:C13" si="1">((+O3*COS($N$3)-P3*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-163.39745962155612</v>
+        <v>-126.60254037844388</v>
       </c>
       <c r="D3" s="71">
         <f t="shared" ref="D3:D13" si="2">((O3*SIN($N$3)+P3*COS($N$3)+$N$9)*$R$4)</f>
-        <v>86.602540378443877</v>
+        <v>84.602540378443877</v>
       </c>
       <c r="E3" s="71">
         <f t="shared" ref="E3:E13" si="3">IF(($R$3*$R$4)=1,1,-1)*(($M3/3.1416*180)+$N$5)</f>
-        <v>30</v>
+        <v>-30</v>
       </c>
       <c r="F3" s="70">
         <v>5</v>
       </c>
       <c r="G3" s="73">
         <f t="shared" ref="G3:G13" si="4">IF($R$3*$R$4=-1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -13765,7 +13770,7 @@
         <v>16</v>
       </c>
       <c r="R3" s="56">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="T3" s="21" t="s">
         <v>18</v>
@@ -13781,22 +13786,22 @@
       </c>
       <c r="C4" s="71">
         <f t="shared" si="1"/>
-        <v>-154.1598553145221</v>
+        <v>-135.8401446854779</v>
       </c>
       <c r="D4" s="71">
         <f t="shared" si="2"/>
-        <v>102.60254037844385</v>
+        <v>100.60254037844385</v>
       </c>
       <c r="E4" s="71">
         <f t="shared" si="3"/>
-        <v>-29.999859694228427</v>
+        <v>29.999859694228427</v>
       </c>
       <c r="F4" s="70">
         <v>5</v>
       </c>
       <c r="G4" s="73">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -13839,22 +13844,22 @@
       </c>
       <c r="C5" s="71">
         <f t="shared" si="1"/>
-        <v>-135.6846467004541</v>
+        <v>-154.3153532995459</v>
       </c>
       <c r="D5" s="71">
         <f t="shared" si="2"/>
-        <v>102.60254037844385</v>
+        <v>100.60254037844385</v>
       </c>
       <c r="E5" s="71">
         <f t="shared" si="3"/>
-        <v>-89.999719388456853</v>
+        <v>89.999719388456853</v>
       </c>
       <c r="F5" s="70">
         <v>5</v>
       </c>
       <c r="G5" s="73">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -13896,22 +13901,22 @@
       </c>
       <c r="C6" s="71">
         <f t="shared" si="1"/>
-        <v>-126.44704239342006</v>
+        <v>-163.55295760657992</v>
       </c>
       <c r="D6" s="71">
         <f t="shared" si="2"/>
-        <v>118.60254037844385</v>
+        <v>116.60254037844385</v>
       </c>
       <c r="E6" s="71">
         <f t="shared" si="3"/>
-        <v>-29.999859694228427</v>
+        <v>29.999859694228427</v>
       </c>
       <c r="F6" s="70">
         <v>5</v>
       </c>
       <c r="G6" s="73">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -13951,22 +13956,22 @@
       </c>
       <c r="C7" s="71">
         <f t="shared" si="1"/>
-        <v>-135.68464670045407</v>
+        <v>-154.31535329954593</v>
       </c>
       <c r="D7" s="71">
         <f t="shared" si="2"/>
-        <v>134.60254037844382</v>
+        <v>132.60254037844382</v>
       </c>
       <c r="E7" s="71">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>-30</v>
       </c>
       <c r="F7" s="70">
         <v>5</v>
       </c>
       <c r="G7" s="73">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -13983,7 +13988,7 @@
         <v>0</v>
       </c>
       <c r="N7" s="3">
-        <v>-200</v>
+        <v>90</v>
       </c>
       <c r="O7" s="46">
         <v>148</v>
@@ -14005,22 +14010,22 @@
       </c>
       <c r="C8" s="71">
         <f t="shared" si="1"/>
-        <v>-126.44704239342002</v>
+        <v>-163.55295760657998</v>
       </c>
       <c r="D8" s="71">
         <f t="shared" si="2"/>
-        <v>150.60254037844379</v>
+        <v>148.60254037844379</v>
       </c>
       <c r="E8" s="71">
         <f t="shared" si="3"/>
-        <v>-29.999859694228427</v>
+        <v>29.999859694228427</v>
       </c>
       <c r="F8" s="70">
         <v>5</v>
       </c>
       <c r="G8" s="73">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -14059,22 +14064,22 @@
       </c>
       <c r="C9" s="71">
         <f t="shared" si="1"/>
-        <v>-135.68464670045404</v>
+        <v>-154.31535329954596</v>
       </c>
       <c r="D9" s="71">
         <f t="shared" si="2"/>
-        <v>166.60254037844379</v>
+        <v>164.60254037844379</v>
       </c>
       <c r="E9" s="71">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>-30</v>
       </c>
       <c r="F9" s="70">
         <v>5</v>
       </c>
       <c r="G9" s="73">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="43">
@@ -14090,7 +14095,7 @@
         <v>0</v>
       </c>
       <c r="N9" s="3">
-        <v>-50</v>
+        <v>-52</v>
       </c>
       <c r="O9" s="46">
         <v>164</v>
@@ -14110,22 +14115,22 @@
       </c>
       <c r="C10" s="71">
         <f t="shared" si="1"/>
-        <v>-154.15985531452205</v>
+        <v>-135.84014468547795</v>
       </c>
       <c r="D10" s="71">
         <f t="shared" si="2"/>
-        <v>166.60254037844379</v>
+        <v>164.60254037844379</v>
       </c>
       <c r="E10" s="71">
         <f t="shared" si="3"/>
-        <v>89.999859694228434</v>
+        <v>-89.999859694228434</v>
       </c>
       <c r="F10" s="70">
         <v>5</v>
       </c>
       <c r="G10" s="73">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="43">
@@ -14160,22 +14165,22 @@
       </c>
       <c r="C11" s="71">
         <f t="shared" si="1"/>
-        <v>-163.3974596215561</v>
+        <v>-126.6025403784439</v>
       </c>
       <c r="D11" s="71">
         <f t="shared" si="2"/>
-        <v>118.60254037844382</v>
+        <v>116.60254037844382</v>
       </c>
       <c r="E11" s="71">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>-30</v>
       </c>
       <c r="F11" s="70">
         <v>5</v>
       </c>
       <c r="G11" s="73">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="43">
@@ -14211,22 +14216,22 @@
       </c>
       <c r="C12" s="71">
         <f t="shared" si="1"/>
-        <v>-154.15985531452208</v>
+        <v>-135.84014468547792</v>
       </c>
       <c r="D12" s="71">
         <f t="shared" si="2"/>
-        <v>134.60254037844379</v>
+        <v>132.60254037844379</v>
       </c>
       <c r="E12" s="71">
         <f t="shared" si="3"/>
-        <v>-29.999859694228427</v>
+        <v>29.999859694228427</v>
       </c>
       <c r="F12" s="70">
         <v>5</v>
       </c>
       <c r="G12" s="73">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="43">
@@ -14259,22 +14264,22 @@
       </c>
       <c r="C13" s="71">
         <f t="shared" si="1"/>
-        <v>-163.3974596215561</v>
+        <v>-126.60254037844392</v>
       </c>
       <c r="D13" s="71">
         <f t="shared" si="2"/>
-        <v>150.60254037844379</v>
+        <v>148.60254037844379</v>
       </c>
       <c r="E13" s="71">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>-30</v>
       </c>
       <c r="F13" s="70">
         <v>5</v>
       </c>
       <c r="G13" s="73">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="43">
@@ -14660,7 +14665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
@@ -14911,7 +14916,7 @@
         <v>0</v>
       </c>
       <c r="N7" s="3">
-        <v>-184</v>
+        <v>-186</v>
       </c>
       <c r="O7" s="46">
         <v>148</v>
@@ -14980,7 +14985,7 @@
         <v>0</v>
       </c>
       <c r="N9" s="3">
-        <v>-100</v>
+        <v>-110</v>
       </c>
       <c r="O9" s="46">
         <v>164</v>
@@ -15063,11 +15068,11 @@
       </c>
       <c r="C12" s="71">
         <f>((+O12*COS($N$3)-P12*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-52</v>
+        <v>-54</v>
       </c>
       <c r="D12" s="71">
         <f>((O12*SIN($N$3)+P12*COS($N$3)+$N$9)*$R$4)</f>
-        <v>36.95041722813599</v>
+        <v>26.95041722813599</v>
       </c>
       <c r="E12" s="71">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M12/3.1416*180)+$N$5)</f>
@@ -15111,11 +15116,11 @@
       </c>
       <c r="C13" s="71">
         <f>((+O13*COS($N$3)-P13*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-52</v>
+        <v>-54</v>
       </c>
       <c r="D13" s="71">
         <f>((O13*SIN($N$3)+P13*COS($N$3)+$N$9)*$R$4)</f>
-        <v>55.425625842203999</v>
+        <v>45.425625842203999</v>
       </c>
       <c r="E13" s="71">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M13/3.1416*180)+$N$5)</f>
@@ -15159,11 +15164,11 @@
       </c>
       <c r="C14" s="71">
         <f>((+O14*COS($N$3)-P14*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-68</v>
+        <v>-70</v>
       </c>
       <c r="D14" s="71">
         <f>((O14*SIN($N$3)+P14*COS($N$3)+$N$9)*$R$4)</f>
-        <v>64.66323014923799</v>
+        <v>54.66323014923799</v>
       </c>
       <c r="E14" s="71">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M14/3.1416*180)+$N$5)</f>
@@ -15323,11 +15328,11 @@
       </c>
       <c r="C19" s="71">
         <f>((+O19*COS($N$3)-P19*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-84</v>
+        <v>-86</v>
       </c>
       <c r="D19" s="71">
         <f>((O19*SIN($N$3)+P19*COS($N$3)+$N$9)*$R$4)</f>
-        <v>55.425625842203999</v>
+        <v>45.425625842203999</v>
       </c>
       <c r="E19" s="71">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M19/3.1416*180)+$N$5)</f>
@@ -15371,11 +15376,11 @@
       </c>
       <c r="C20" s="71">
         <f>((+O20*COS($N$3)-P20*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-100</v>
+        <v>-102</v>
       </c>
       <c r="D20" s="71">
         <f>((O20*SIN($N$3)+P20*COS($N$3)+$N$9)*$R$4)</f>
-        <v>64.66323014923799</v>
+        <v>54.66323014923799</v>
       </c>
       <c r="E20" s="71">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M20/3.1416*180)+$N$5)</f>
@@ -15419,11 +15424,11 @@
       </c>
       <c r="C21" s="71">
         <f>((+O21*COS($N$3)-P21*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-116</v>
+        <v>-118</v>
       </c>
       <c r="D21" s="71">
         <f>((O21*SIN($N$3)+P21*COS($N$3)+$N$9)*$R$4)</f>
-        <v>55.425625842203999</v>
+        <v>45.425625842203999</v>
       </c>
       <c r="E21" s="71">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M21/3.1416*180)+$N$5)</f>
@@ -15467,11 +15472,11 @@
       </c>
       <c r="C22" s="71">
         <f>((+O22*COS($N$3)-P22*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-116</v>
+        <v>-118</v>
       </c>
       <c r="D22" s="71">
         <f>((O22*SIN($N$3)+P22*COS($N$3)+$N$9)*$R$4)</f>
-        <v>36.95041722813599</v>
+        <v>26.95041722813599</v>
       </c>
       <c r="E22" s="71">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M22/3.1416*180)+$N$5)</f>
@@ -15515,11 +15520,11 @@
       </c>
       <c r="C23" s="71">
         <f>((+O23*COS($N$3)-P23*SIN($N$3)+$N$7)*$R$3)</f>
-        <v>-84</v>
+        <v>-86</v>
       </c>
       <c r="D23" s="71">
         <f>((O23*SIN($N$3)+P23*COS($N$3)+$N$9)*$R$4)</f>
-        <v>36.95041722813599</v>
+        <v>26.95041722813599</v>
       </c>
       <c r="E23" s="71">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M23/3.1416*180)+$N$5)</f>
@@ -15626,8 +15631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G94" sqref="A3:G94"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:G94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15702,7 +15707,7 @@
       </c>
       <c r="C4" s="79">
         <f>IF(lower!C4="", "", lower!C4)</f>
-        <v>-103.92225100748811</v>
+        <v>-67.077748992511886</v>
       </c>
       <c r="D4" s="79">
         <f>IF(lower!D4="", "", lower!D4)</f>
@@ -15710,7 +15715,7 @@
       </c>
       <c r="E4" s="79">
         <f>IF(lower!E4="", "", lower!E4)</f>
-        <v>-89.999859694228434</v>
+        <v>89.999859694228434</v>
       </c>
       <c r="F4" s="74">
         <f>IF(lower!F4=0, "", lower!F4)</f>
@@ -15718,7 +15723,7 @@
       </c>
       <c r="G4" s="74">
         <f>IF(lower!$A4="", "", lower!G4)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -15732,7 +15737,7 @@
       </c>
       <c r="C5" s="79">
         <f>IF(lower!C5="", "", lower!C5)</f>
-        <v>-94.684646700454095</v>
+        <v>-76.315353299545905</v>
       </c>
       <c r="D5" s="79">
         <f>IF(lower!D5="", "", lower!D5)</f>
@@ -15740,7 +15745,7 @@
       </c>
       <c r="E5" s="79">
         <f>IF(lower!E5="", "", lower!E5)</f>
-        <v>-149.99971938845687</v>
+        <v>149.99971938845687</v>
       </c>
       <c r="F5" s="74">
         <f>IF(lower!F5=0, "", lower!F5)</f>
@@ -15748,7 +15753,7 @@
       </c>
       <c r="G5" s="74">
         <f>IF(lower!$A5="", "", lower!G5)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -15762,7 +15767,7 @@
       </c>
       <c r="C6" s="79">
         <f>IF(lower!C6="", "", lower!C6)</f>
-        <v>-76.209438086386058</v>
+        <v>-94.790561913613942</v>
       </c>
       <c r="D6" s="79">
         <f>IF(lower!D6="", "", lower!D6)</f>
@@ -15770,7 +15775,7 @@
       </c>
       <c r="E6" s="79">
         <f>IF(lower!E6="", "", lower!E6)</f>
-        <v>-89.999859694228434</v>
+        <v>89.999859694228434</v>
       </c>
       <c r="F6" s="74">
         <f>IF(lower!F6=0, "", lower!F6)</f>
@@ -15778,7 +15783,7 @@
       </c>
       <c r="G6" s="74">
         <f>IF(lower!$A6="", "", lower!G6)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -15792,7 +15797,7 @@
       </c>
       <c r="C7" s="79">
         <f>IF(lower!C7="", "", lower!C7)</f>
-        <v>-66.971833779352067</v>
+        <v>-104.02816622064793</v>
       </c>
       <c r="D7" s="79">
         <f>IF(lower!D7="", "", lower!D7)</f>
@@ -15800,7 +15805,7 @@
       </c>
       <c r="E7" s="79">
         <f>IF(lower!E7="", "", lower!E7)</f>
-        <v>-30</v>
+        <v>30</v>
       </c>
       <c r="F7" s="74">
         <f>IF(lower!F7=0, "", lower!F7)</f>
@@ -15808,7 +15813,7 @@
       </c>
       <c r="G7" s="74">
         <f>IF(lower!$A7="", "", lower!G7)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -15912,7 +15917,7 @@
       </c>
       <c r="C11" s="79">
         <f>IF(lower!C11="", "", lower!C11)</f>
-        <v>-94.684646700454124</v>
+        <v>-76.315353299545876</v>
       </c>
       <c r="D11" s="79">
         <f>IF(lower!D11="", "", lower!D11)</f>
@@ -15920,7 +15925,7 @@
       </c>
       <c r="E11" s="79">
         <f>IF(lower!E11="", "", lower!E11)</f>
-        <v>-30</v>
+        <v>30</v>
       </c>
       <c r="F11" s="74">
         <f>IF(lower!F11=0, "", lower!F11)</f>
@@ -15928,7 +15933,7 @@
       </c>
       <c r="G11" s="74">
         <f>IF(lower!$A11="", "", lower!G11)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -15942,7 +15947,7 @@
       </c>
       <c r="C12" s="79">
         <f>IF(lower!C12="", "", lower!C12)</f>
-        <v>-76.209438086386115</v>
+        <v>-94.790561913613885</v>
       </c>
       <c r="D12" s="79">
         <f>IF(lower!D12="", "", lower!D12)</f>
@@ -15950,7 +15955,7 @@
       </c>
       <c r="E12" s="79">
         <f>IF(lower!E12="", "", lower!E12)</f>
-        <v>-89.999859694228434</v>
+        <v>89.999859694228434</v>
       </c>
       <c r="F12" s="74">
         <f>IF(lower!F12=0, "", lower!F12)</f>
@@ -15958,7 +15963,7 @@
       </c>
       <c r="G12" s="74">
         <f>IF(lower!$A12="", "", lower!G12)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -15972,7 +15977,7 @@
       </c>
       <c r="C13" s="79">
         <f>IF(lower!C13="", "", lower!C13)</f>
-        <v>-66.971833779352096</v>
+        <v>-104.0281662206479</v>
       </c>
       <c r="D13" s="79">
         <f>IF(lower!D13="", "", lower!D13)</f>
@@ -15980,7 +15985,7 @@
       </c>
       <c r="E13" s="79">
         <f>IF(lower!E13="", "", lower!E13)</f>
-        <v>-30</v>
+        <v>30</v>
       </c>
       <c r="F13" s="74">
         <f>IF(lower!F13=0, "", lower!F13)</f>
@@ -15988,7 +15993,7 @@
       </c>
       <c r="G13" s="74">
         <f>IF(lower!$A13="", "", lower!G13)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -16002,7 +16007,7 @@
       </c>
       <c r="C14" s="79">
         <f>IF(lower!C14="", "", lower!C14)</f>
-        <v>-76.209438086386115</v>
+        <v>-94.790561913613885</v>
       </c>
       <c r="D14" s="79">
         <f>IF(lower!D14="", "", lower!D14)</f>
@@ -16010,7 +16015,7 @@
       </c>
       <c r="E14" s="79">
         <f>IF(lower!E14="", "", lower!E14)</f>
-        <v>29.999859694228427</v>
+        <v>-29.999859694228427</v>
       </c>
       <c r="F14" s="74">
         <f>IF(lower!F14=0, "", lower!F14)</f>
@@ -16018,7 +16023,7 @@
       </c>
       <c r="G14" s="74">
         <f>IF(lower!$A14="", "", lower!G14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -16152,7 +16157,7 @@
       </c>
       <c r="C19" s="79">
         <f>IF(lower!C19="", "", lower!C19)</f>
-        <v>-94.684646700454152</v>
+        <v>-76.315353299545848</v>
       </c>
       <c r="D19" s="79">
         <f>IF(lower!D19="", "", lower!D19)</f>
@@ -16160,7 +16165,7 @@
       </c>
       <c r="E19" s="79">
         <f>IF(lower!E19="", "", lower!E19)</f>
-        <v>89.999719388456853</v>
+        <v>-89.999719388456853</v>
       </c>
       <c r="F19" s="74">
         <f>IF(lower!F19=0, "", lower!F19)</f>
@@ -16168,7 +16173,7 @@
       </c>
       <c r="G19" s="74">
         <f>IF(lower!$A19="", "", lower!G19)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -16272,7 +16277,7 @@
       </c>
       <c r="C23" s="79">
         <f>IF(lower!C23="", "", lower!C23)</f>
-        <v>-103.92225100748814</v>
+        <v>-67.077748992511857</v>
       </c>
       <c r="D23" s="79">
         <f>IF(lower!D23="", "", lower!D23)</f>
@@ -16280,7 +16285,7 @@
       </c>
       <c r="E23" s="79">
         <f>IF(lower!E23="", "", lower!E23)</f>
-        <v>149.99957908268468</v>
+        <v>-149.99957908268468</v>
       </c>
       <c r="F23" s="74">
         <f>IF(lower!F23=0, "", lower!F23)</f>
@@ -16288,7 +16293,7 @@
       </c>
       <c r="G23" s="74">
         <f>IF(lower!$A23="", "", lower!G23)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -16362,15 +16367,15 @@
       </c>
       <c r="C26" s="68">
         <f>IF(external!C3="", "", external!C3)</f>
-        <v>-36.602540378443848</v>
+        <v>-16.397459621556152</v>
       </c>
       <c r="D26" s="68">
         <f>IF(external!D3="", "", external!D3)</f>
-        <v>161.39745962155612</v>
+        <v>163.39745962155612</v>
       </c>
       <c r="E26" s="68">
         <f>IF(external!E3="", "", external!E3)</f>
-        <v>210</v>
+        <v>-210</v>
       </c>
       <c r="F26" s="63">
         <f>IF(external!F3="", "", external!F3)</f>
@@ -16378,7 +16383,7 @@
       </c>
       <c r="G26" s="63">
         <f>IF(external!A3="", "", external!G3)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -16392,15 +16397,15 @@
       </c>
       <c r="C27" s="68">
         <f>IF(external!C4="", "", external!C4)</f>
-        <v>-45.84014468547786</v>
+        <v>-7.1598553145221402</v>
       </c>
       <c r="D27" s="68">
         <f>IF(external!D4="", "", external!D4)</f>
-        <v>145.39745962155615</v>
+        <v>147.39745962155615</v>
       </c>
       <c r="E27" s="68">
         <f>IF(external!E4="", "", external!E4)</f>
-        <v>150.00014030577157</v>
+        <v>-150.00014030577157</v>
       </c>
       <c r="F27" s="63">
         <f>IF(external!F4="", "", external!F4)</f>
@@ -16408,7 +16413,7 @@
       </c>
       <c r="G27" s="63">
         <f>IF(external!A4="", "", external!G4)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -16602,15 +16607,15 @@
       </c>
       <c r="C34" s="68">
         <f>IF(external!C11="", "", external!C11)</f>
-        <v>-36.602540378443862</v>
+        <v>-16.397459621556138</v>
       </c>
       <c r="D34" s="68">
         <f>IF(external!D11="", "", external!D11)</f>
-        <v>129.39745962155615</v>
+        <v>131.39745962155615</v>
       </c>
       <c r="E34" s="68">
         <f>IF(external!E11="", "", external!E11)</f>
-        <v>210</v>
+        <v>-210</v>
       </c>
       <c r="F34" s="63">
         <f>IF(external!F11="", "", external!F11)</f>
@@ -16618,7 +16623,7 @@
       </c>
       <c r="G34" s="63">
         <f>IF(external!A11="", "", external!G11)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -16632,15 +16637,15 @@
       </c>
       <c r="C35" s="68">
         <f>IF(external!C12="", "", external!C12)</f>
-        <v>-45.840144685477881</v>
+        <v>-7.1598553145221189</v>
       </c>
       <c r="D35" s="68">
         <f>IF(external!D12="", "", external!D12)</f>
-        <v>113.39745962155618</v>
+        <v>115.39745962155618</v>
       </c>
       <c r="E35" s="68">
         <f>IF(external!E12="", "", external!E12)</f>
-        <v>150.00014030577157</v>
+        <v>-150.00014030577157</v>
       </c>
       <c r="F35" s="63">
         <f>IF(external!F12="", "", external!F12)</f>
@@ -16648,7 +16653,7 @@
       </c>
       <c r="G35" s="63">
         <f>IF(external!A12="", "", external!G12)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -16662,15 +16667,15 @@
       </c>
       <c r="C36" s="68">
         <f>IF(external!C13="", "", external!C13)</f>
-        <v>-36.602540378443877</v>
+        <v>-16.397459621556123</v>
       </c>
       <c r="D36" s="68">
         <f>IF(external!D13="", "", external!D13)</f>
-        <v>97.397459621556209</v>
+        <v>99.397459621556209</v>
       </c>
       <c r="E36" s="68">
         <f>IF(external!E13="", "", external!E13)</f>
-        <v>210</v>
+        <v>-210</v>
       </c>
       <c r="F36" s="63">
         <f>IF(external!F13="", "", external!F13)</f>
@@ -16678,7 +16683,7 @@
       </c>
       <c r="G36" s="63">
         <f>IF(external!A13="", "", external!G13)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -16692,15 +16697,15 @@
       </c>
       <c r="C37" s="68">
         <f>IF(external!C14="", "", external!C14)</f>
-        <v>-18.127331764375867</v>
+        <v>-34.872668235624133</v>
       </c>
       <c r="D37" s="68">
         <f>IF(external!D14="", "", external!D14)</f>
-        <v>97.397459621556209</v>
+        <v>99.397459621556209</v>
       </c>
       <c r="E37" s="68">
         <f>IF(external!E14="", "", external!E14)</f>
-        <v>269.99985969422841</v>
+        <v>-269.99985969422841</v>
       </c>
       <c r="F37" s="63">
         <f>IF(external!F14="", "", external!F14)</f>
@@ -16708,7 +16713,7 @@
       </c>
       <c r="G37" s="63">
         <f>IF(external!A14="", "", external!G14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -16722,15 +16727,15 @@
       </c>
       <c r="C38" s="68">
         <f>IF(external!C15="", "", external!C15)</f>
-        <v>-8.8897274573418628</v>
+        <v>-44.110272542658137</v>
       </c>
       <c r="D38" s="68">
         <f>IF(external!D15="", "", external!D15)</f>
-        <v>81.397459621556209</v>
+        <v>83.397459621556209</v>
       </c>
       <c r="E38" s="68">
         <f>IF(external!E15="", "", external!E15)</f>
-        <v>210</v>
+        <v>-210</v>
       </c>
       <c r="F38" s="63">
         <f>IF(external!F15="", "", external!F15)</f>
@@ -16738,7 +16743,7 @@
       </c>
       <c r="G38" s="63">
         <f>IF(external!A15="", "", external!G15)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -16842,15 +16847,15 @@
       </c>
       <c r="C42" s="68">
         <f>IF(external!C19="", "", external!C19)</f>
-        <v>-8.8897274573418485</v>
+        <v>-44.110272542658151</v>
       </c>
       <c r="D42" s="68">
         <f>IF(external!D19="", "", external!D19)</f>
-        <v>113.39745962155621</v>
+        <v>115.39745962155621</v>
       </c>
       <c r="E42" s="68">
         <f>IF(external!E19="", "", external!E19)</f>
-        <v>329.99971938845687</v>
+        <v>-329.99971938845687</v>
       </c>
       <c r="F42" s="63">
         <f>IF(external!F19="", "", external!F19)</f>
@@ -16858,7 +16863,7 @@
       </c>
       <c r="G42" s="63">
         <f>IF(external!A19="", "", external!G19)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -16962,15 +16967,15 @@
       </c>
       <c r="C46" s="68">
         <f>IF(external!C23="", "", external!C23)</f>
-        <v>-18.127331764375853</v>
+        <v>-34.872668235624147</v>
       </c>
       <c r="D46" s="68">
         <f>IF(external!D23="", "", external!D23)</f>
-        <v>129.39745962155618</v>
+        <v>131.39745962155618</v>
       </c>
       <c r="E46" s="68">
         <f>IF(external!E23="", "", external!E23)</f>
-        <v>389.9995790826847</v>
+        <v>-389.9995790826847</v>
       </c>
       <c r="F46" s="63">
         <f>IF(external!F23="", "", external!F23)</f>
@@ -16978,7 +16983,7 @@
       </c>
       <c r="G46" s="63">
         <f>IF(external!A23="", "", external!G23)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -16992,15 +16997,15 @@
       </c>
       <c r="C47" s="68">
         <f>IF(external!C24="", "", external!C24)</f>
-        <v>-8.8897274573418343</v>
+        <v>-44.110272542658166</v>
       </c>
       <c r="D47" s="68">
         <f>IF(external!D24="", "", external!D24)</f>
-        <v>145.39745962155618</v>
+        <v>147.39745962155618</v>
       </c>
       <c r="E47" s="68">
         <f>IF(external!E24="", "", external!E24)</f>
-        <v>329.99971938845687</v>
+        <v>-329.99971938845687</v>
       </c>
       <c r="F47" s="63">
         <f>IF(external!F24="", "", external!F24)</f>
@@ -17008,7 +17013,7 @@
       </c>
       <c r="G47" s="63">
         <f>IF(external!A24="", "", external!G24)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -17022,15 +17027,15 @@
       </c>
       <c r="C48" s="68">
         <f>IF(external!C25="", "", external!C25)</f>
-        <v>-18.127331764375832</v>
+        <v>-34.872668235624168</v>
       </c>
       <c r="D48" s="68">
         <f>IF(external!D25="", "", external!D25)</f>
-        <v>161.39745962155615</v>
+        <v>163.39745962155615</v>
       </c>
       <c r="E48" s="68">
         <f>IF(external!E25="", "", external!E25)</f>
-        <v>389.9995790826847</v>
+        <v>-389.9995790826847</v>
       </c>
       <c r="F48" s="63">
         <f>IF(external!F25="", "", external!F25)</f>
@@ -17038,7 +17043,7 @@
       </c>
       <c r="G48" s="63">
         <f>IF(external!A25="", "", external!G25)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -17052,15 +17057,15 @@
       </c>
       <c r="C49" s="69">
         <f>IF(internal!C3="", "", internal!C3)</f>
-        <v>-163.39745962155612</v>
+        <v>-126.60254037844388</v>
       </c>
       <c r="D49" s="69">
         <f>IF(internal!D3="", "", internal!D3)</f>
-        <v>86.602540378443877</v>
+        <v>84.602540378443877</v>
       </c>
       <c r="E49" s="69">
         <f>IF(internal!E3="", "", internal!E3)</f>
-        <v>30</v>
+        <v>-30</v>
       </c>
       <c r="F49" s="62">
         <f>IF(internal!F3="", "", internal!F3)</f>
@@ -17068,7 +17073,7 @@
       </c>
       <c r="G49" s="62">
         <f>IF(internal!A3="", "", internal!G3)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -17082,15 +17087,15 @@
       </c>
       <c r="C50" s="69">
         <f>IF(internal!C4="", "", internal!C4)</f>
-        <v>-154.1598553145221</v>
+        <v>-135.8401446854779</v>
       </c>
       <c r="D50" s="69">
         <f>IF(internal!D4="", "", internal!D4)</f>
-        <v>102.60254037844385</v>
+        <v>100.60254037844385</v>
       </c>
       <c r="E50" s="69">
         <f>IF(internal!E4="", "", internal!E4)</f>
-        <v>-29.999859694228427</v>
+        <v>29.999859694228427</v>
       </c>
       <c r="F50" s="62">
         <f>IF(internal!F4="", "", internal!F4)</f>
@@ -17098,7 +17103,7 @@
       </c>
       <c r="G50" s="62">
         <f>IF(internal!A4="", "", internal!G4)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -17112,15 +17117,15 @@
       </c>
       <c r="C51" s="69">
         <f>IF(internal!C5="", "", internal!C5)</f>
-        <v>-135.6846467004541</v>
+        <v>-154.3153532995459</v>
       </c>
       <c r="D51" s="69">
         <f>IF(internal!D5="", "", internal!D5)</f>
-        <v>102.60254037844385</v>
+        <v>100.60254037844385</v>
       </c>
       <c r="E51" s="69">
         <f>IF(internal!E5="", "", internal!E5)</f>
-        <v>-89.999719388456853</v>
+        <v>89.999719388456853</v>
       </c>
       <c r="F51" s="62">
         <f>IF(internal!F5="", "", internal!F5)</f>
@@ -17128,7 +17133,7 @@
       </c>
       <c r="G51" s="62">
         <f>IF(internal!A5="", "", internal!G5)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -17142,15 +17147,15 @@
       </c>
       <c r="C52" s="69">
         <f>IF(internal!C6="", "", internal!C6)</f>
-        <v>-126.44704239342006</v>
+        <v>-163.55295760657992</v>
       </c>
       <c r="D52" s="69">
         <f>IF(internal!D6="", "", internal!D6)</f>
-        <v>118.60254037844385</v>
+        <v>116.60254037844385</v>
       </c>
       <c r="E52" s="69">
         <f>IF(internal!E6="", "", internal!E6)</f>
-        <v>-29.999859694228427</v>
+        <v>29.999859694228427</v>
       </c>
       <c r="F52" s="62">
         <f>IF(internal!F6="", "", internal!F6)</f>
@@ -17158,7 +17163,7 @@
       </c>
       <c r="G52" s="62">
         <f>IF(internal!A6="", "", internal!G6)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -17172,15 +17177,15 @@
       </c>
       <c r="C53" s="69">
         <f>IF(internal!C7="", "", internal!C7)</f>
-        <v>-135.68464670045407</v>
+        <v>-154.31535329954593</v>
       </c>
       <c r="D53" s="69">
         <f>IF(internal!D7="", "", internal!D7)</f>
-        <v>134.60254037844382</v>
+        <v>132.60254037844382</v>
       </c>
       <c r="E53" s="69">
         <f>IF(internal!E7="", "", internal!E7)</f>
-        <v>30</v>
+        <v>-30</v>
       </c>
       <c r="F53" s="62">
         <f>IF(internal!F7="", "", internal!F7)</f>
@@ -17188,7 +17193,7 @@
       </c>
       <c r="G53" s="62">
         <f>IF(internal!A7="", "", internal!G7)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -17202,15 +17207,15 @@
       </c>
       <c r="C54" s="69">
         <f>IF(internal!C8="", "", internal!C8)</f>
-        <v>-126.44704239342002</v>
+        <v>-163.55295760657998</v>
       </c>
       <c r="D54" s="69">
         <f>IF(internal!D8="", "", internal!D8)</f>
-        <v>150.60254037844379</v>
+        <v>148.60254037844379</v>
       </c>
       <c r="E54" s="69">
         <f>IF(internal!E8="", "", internal!E8)</f>
-        <v>-29.999859694228427</v>
+        <v>29.999859694228427</v>
       </c>
       <c r="F54" s="62">
         <f>IF(internal!F8="", "", internal!F8)</f>
@@ -17218,7 +17223,7 @@
       </c>
       <c r="G54" s="62">
         <f>IF(internal!A8="", "", internal!G8)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -17232,15 +17237,15 @@
       </c>
       <c r="C55" s="69">
         <f>IF(internal!C9="", "", internal!C9)</f>
-        <v>-135.68464670045404</v>
+        <v>-154.31535329954596</v>
       </c>
       <c r="D55" s="69">
         <f>IF(internal!D9="", "", internal!D9)</f>
-        <v>166.60254037844379</v>
+        <v>164.60254037844379</v>
       </c>
       <c r="E55" s="69">
         <f>IF(internal!E9="", "", internal!E9)</f>
-        <v>30</v>
+        <v>-30</v>
       </c>
       <c r="F55" s="62">
         <f>IF(internal!F9="", "", internal!F9)</f>
@@ -17248,7 +17253,7 @@
       </c>
       <c r="G55" s="62">
         <f>IF(internal!A9="", "", internal!G9)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -17262,15 +17267,15 @@
       </c>
       <c r="C56" s="69">
         <f>IF(internal!C10="", "", internal!C10)</f>
-        <v>-154.15985531452205</v>
+        <v>-135.84014468547795</v>
       </c>
       <c r="D56" s="69">
         <f>IF(internal!D10="", "", internal!D10)</f>
-        <v>166.60254037844379</v>
+        <v>164.60254037844379</v>
       </c>
       <c r="E56" s="69">
         <f>IF(internal!E10="", "", internal!E10)</f>
-        <v>89.999859694228434</v>
+        <v>-89.999859694228434</v>
       </c>
       <c r="F56" s="62">
         <f>IF(internal!F10="", "", internal!F10)</f>
@@ -17278,7 +17283,7 @@
       </c>
       <c r="G56" s="62">
         <f>IF(internal!A10="", "", internal!G10)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -17292,15 +17297,15 @@
       </c>
       <c r="C57" s="69">
         <f>IF(internal!C11="", "", internal!C11)</f>
-        <v>-163.3974596215561</v>
+        <v>-126.6025403784439</v>
       </c>
       <c r="D57" s="69">
         <f>IF(internal!D11="", "", internal!D11)</f>
-        <v>118.60254037844382</v>
+        <v>116.60254037844382</v>
       </c>
       <c r="E57" s="69">
         <f>IF(internal!E11="", "", internal!E11)</f>
-        <v>30</v>
+        <v>-30</v>
       </c>
       <c r="F57" s="62">
         <f>IF(internal!F11="", "", internal!F11)</f>
@@ -17308,7 +17313,7 @@
       </c>
       <c r="G57" s="62">
         <f>IF(internal!A11="", "", internal!G11)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -17322,15 +17327,15 @@
       </c>
       <c r="C58" s="69">
         <f>IF(internal!C12="", "", internal!C12)</f>
-        <v>-154.15985531452208</v>
+        <v>-135.84014468547792</v>
       </c>
       <c r="D58" s="69">
         <f>IF(internal!D12="", "", internal!D12)</f>
-        <v>134.60254037844379</v>
+        <v>132.60254037844379</v>
       </c>
       <c r="E58" s="69">
         <f>IF(internal!E12="", "", internal!E12)</f>
-        <v>-29.999859694228427</v>
+        <v>29.999859694228427</v>
       </c>
       <c r="F58" s="62">
         <f>IF(internal!F12="", "", internal!F12)</f>
@@ -17338,7 +17343,7 @@
       </c>
       <c r="G58" s="62">
         <f>IF(internal!A12="", "", internal!G12)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -17352,15 +17357,15 @@
       </c>
       <c r="C59" s="69">
         <f>IF(internal!C13="", "", internal!C13)</f>
-        <v>-163.3974596215561</v>
+        <v>-126.60254037844392</v>
       </c>
       <c r="D59" s="69">
         <f>IF(internal!D13="", "", internal!D13)</f>
-        <v>150.60254037844379</v>
+        <v>148.60254037844379</v>
       </c>
       <c r="E59" s="69">
         <f>IF(internal!E13="", "", internal!E13)</f>
-        <v>30</v>
+        <v>-30</v>
       </c>
       <c r="F59" s="62">
         <f>IF(internal!F13="", "", internal!F13)</f>
@@ -17368,7 +17373,7 @@
       </c>
       <c r="G59" s="62">
         <f>IF(internal!A13="", "", internal!G13)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -18012,11 +18017,11 @@
       </c>
       <c r="C81" s="80">
         <f>IF(upper!C12="", "", upper!C12)</f>
-        <v>-52</v>
+        <v>-54</v>
       </c>
       <c r="D81" s="80">
         <f>IF(upper!D12="", "", upper!D12)</f>
-        <v>36.95041722813599</v>
+        <v>26.95041722813599</v>
       </c>
       <c r="E81" s="80">
         <f>IF(upper!E12="", "", upper!E12)</f>
@@ -18042,11 +18047,11 @@
       </c>
       <c r="C82" s="80">
         <f>IF(upper!C13="", "", upper!C13)</f>
-        <v>-52</v>
+        <v>-54</v>
       </c>
       <c r="D82" s="80">
         <f>IF(upper!D13="", "", upper!D13)</f>
-        <v>55.425625842203999</v>
+        <v>45.425625842203999</v>
       </c>
       <c r="E82" s="80">
         <f>IF(upper!E13="", "", upper!E13)</f>
@@ -18072,11 +18077,11 @@
       </c>
       <c r="C83" s="80">
         <f>IF(upper!C14="", "", upper!C14)</f>
-        <v>-68</v>
+        <v>-70</v>
       </c>
       <c r="D83" s="80">
         <f>IF(upper!D14="", "", upper!D14)</f>
-        <v>64.66323014923799</v>
+        <v>54.66323014923799</v>
       </c>
       <c r="E83" s="80">
         <f>IF(upper!E14="", "", upper!E14)</f>
@@ -18222,11 +18227,11 @@
       </c>
       <c r="C88" s="80">
         <f>IF(upper!C19="", "", upper!C19)</f>
-        <v>-84</v>
+        <v>-86</v>
       </c>
       <c r="D88" s="80">
         <f>IF(upper!D19="", "", upper!D19)</f>
-        <v>55.425625842203999</v>
+        <v>45.425625842203999</v>
       </c>
       <c r="E88" s="80">
         <f>IF(upper!E19="", "", upper!E19)</f>
@@ -18252,11 +18257,11 @@
       </c>
       <c r="C89" s="80">
         <f>IF(upper!C20="", "", upper!C20)</f>
-        <v>-100</v>
+        <v>-102</v>
       </c>
       <c r="D89" s="80">
         <f>IF(upper!D20="", "", upper!D20)</f>
-        <v>64.66323014923799</v>
+        <v>54.66323014923799</v>
       </c>
       <c r="E89" s="80">
         <f>IF(upper!E20="", "", upper!E20)</f>
@@ -18282,11 +18287,11 @@
       </c>
       <c r="C90" s="80">
         <f>IF(upper!C21="", "", upper!C21)</f>
-        <v>-116</v>
+        <v>-118</v>
       </c>
       <c r="D90" s="80">
         <f>IF(upper!D21="", "", upper!D21)</f>
-        <v>55.425625842203999</v>
+        <v>45.425625842203999</v>
       </c>
       <c r="E90" s="80">
         <f>IF(upper!E21="", "", upper!E21)</f>
@@ -18312,11 +18317,11 @@
       </c>
       <c r="C91" s="80">
         <f>IF(upper!C22="", "", upper!C22)</f>
-        <v>-116</v>
+        <v>-118</v>
       </c>
       <c r="D91" s="80">
         <f>IF(upper!D22="", "", upper!D22)</f>
-        <v>36.95041722813599</v>
+        <v>26.95041722813599</v>
       </c>
       <c r="E91" s="80">
         <f>IF(upper!E22="", "", upper!E22)</f>
@@ -18342,11 +18347,11 @@
       </c>
       <c r="C92" s="80">
         <f>IF(upper!C23="", "", upper!C23)</f>
-        <v>-84</v>
+        <v>-86</v>
       </c>
       <c r="D92" s="80">
         <f>IF(upper!D23="", "", upper!D23)</f>
-        <v>36.95041722813599</v>
+        <v>26.95041722813599</v>
       </c>
       <c r="E92" s="80">
         <f>IF(upper!E23="", "", upper!E23)</f>

</xml_diff>